<commit_message>
second commit - updated Dashboard page, DashboardPageTest
</commit_message>
<xml_diff>
--- a/src/main/java/com/salesforce/qa/testdata/SalesforceProjectTestData.xlsx
+++ b/src/main/java/com/salesforce/qa/testdata/SalesforceProjectTestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thndr\eclipse-workspace\SalesforceProjectTest\src\main\java\com\salesforce\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B319353-FFD9-4013-9D65-3E15009AC5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AE7DCB-7187-4A57-8209-7C94673F4FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="636" yWindow="876" windowWidth="21900" windowHeight="11088" xr2:uid="{2CEAFDB3-5223-4F75-A1C0-5E4B986E3980}"/>
+    <workbookView xWindow="636" yWindow="876" windowWidth="21900" windowHeight="11088" activeTab="1" xr2:uid="{2CEAFDB3-5223-4F75-A1C0-5E4B986E3980}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="DashboardPageTabs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -50,6 +51,57 @@
   </si>
   <si>
     <t>@Temp1234567</t>
+  </si>
+  <si>
+    <t>dashboardPageTabs</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Accounts</t>
+  </si>
+  <si>
+    <t>Contacts</t>
+  </si>
+  <si>
+    <t>Leads</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>Dashboards</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Forecasts</t>
+  </si>
+  <si>
+    <t>Files</t>
+  </si>
+  <si>
+    <t>Quotes</t>
+  </si>
+  <si>
+    <t>Chatter</t>
+  </si>
+  <si>
+    <t>Opportunities</t>
+  </si>
+  <si>
+    <t>List Emails</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -73,7 +125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,6 +135,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -114,11 +172,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B98AB188-72C1-4BBA-B5C5-6FDF1D62C084}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
@@ -496,4 +555,108 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A191BF70-292A-4047-862C-F2407DB36ED3}">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>